<commit_message>
Nononcology smoke test data
</commit_message>
<xml_diff>
--- a/Testdata/LiveSLR_SmokeTest.xlsx
+++ b/Testdata/LiveSLR_SmokeTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7532681-E257-41F1-89F9-586F6A957181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08072395-4D0F-46AE-A393-0B4FB762C20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26C09FF1-B3A3-4547-AFE4-A3356FE600D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -159,27 +159,6 @@
   </si>
   <si>
     <t>intervention_section6_checkbox</t>
-  </si>
-  <si>
-    <t>scenario3</t>
-  </si>
-  <si>
-    <t>scenario4</t>
-  </si>
-  <si>
-    <t>Economic</t>
-  </si>
-  <si>
-    <t>Economic_radio_button</t>
-  </si>
-  <si>
-    <t>StandardExcelReport-NewImportLogic_1-Test_Automation_1-Economic-2023_</t>
-  </si>
-  <si>
-    <t>ExcelReport-NewImportLogic_1-Test_Automation_1-Economic-</t>
-  </si>
-  <si>
-    <t>WordReport-NewImportLogic_1 - Test_Automation_1-Economic-</t>
   </si>
   <si>
     <t>This filter allows you to select one of your project(s) to view. Only one SLR project can be selected at this step.</t>
@@ -555,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344B1479-70F0-4B4E-BC73-42393FEE027A}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +582,7 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -635,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -655,7 +634,7 @@
         <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -675,7 +654,7 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -692,16 +671,16 @@
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -709,113 +688,67 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="I8" t="s">
-        <v>22</v>
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>